<commit_message>
deleted old server updated backend for sql
</commit_message>
<xml_diff>
--- a/ERD for Groupomania.xlsx
+++ b/ERD for Groupomania.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15c141d6a280b1ea/Desktop/gitProjects/repos/Groupomania/index/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15c141d6a280b1ea/Desktop/gitProjects/repos/Groupomania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{796A1241-8C49-4688-A6FB-A7A152299477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{796A1241-8C49-4688-A6FB-A7A152299477}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DB7004CB-621B-4143-A61A-4811BF278ADE}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3600" windowWidth="17400" windowHeight="7875" xr2:uid="{E9C435E5-9C83-49FF-9C3C-DC45B389B114}"/>
+    <workbookView xWindow="9330" yWindow="1800" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E9C435E5-9C83-49FF-9C3C-DC45B389B114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Employee</t>
   </si>
@@ -94,6 +95,54 @@
   </si>
   <si>
     <t>PostName</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>phone nr</t>
+  </si>
+  <si>
+    <t>customer nr</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>Shops</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>staff number</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>sum total</t>
   </si>
 </sst>
 </file>
@@ -115,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,16 +211,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C531DDC-934E-493F-9532-2A86E5B2C2A0}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,20 +551,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="H1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -517,7 +573,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
@@ -526,7 +582,7 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
@@ -535,48 +591,48 @@
       <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="L3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="1"/>
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -587,17 +643,17 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1"/>
       <c r="G5" t="s">
         <v>6</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -605,14 +661,14 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
       <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -620,35 +676,35 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I10" s="4"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I11" s="4"/>
+      <c r="I11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -660,4 +716,84 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D19B2B6-849B-4922-8228-CB3DE83DE016}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>